<commit_message>
Modified native text generation to handle nested if statements.
</commit_message>
<xml_diff>
--- a/For translation.xlsx
+++ b/For translation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -129,24 +129,12 @@
     <t>traveling</t>
   </si>
   <si>
-    <t>painting</t>
-  </si>
-  <si>
-    <t>eating</t>
-  </si>
-  <si>
     <t>rectangle</t>
   </si>
   <si>
     <t>circle</t>
   </si>
   <si>
-    <t>cube</t>
-  </si>
-  <si>
-    <t>sphere</t>
-  </si>
-  <si>
     <t>cost</t>
   </si>
   <si>
@@ -156,42 +144,9 @@
     <t>payment</t>
   </si>
   <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>width</t>
-  </si>
-  <si>
-    <t>radius</t>
-  </si>
-  <si>
-    <t>diameter</t>
-  </si>
-  <si>
-    <t>side</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>body_temperature</t>
-  </si>
-  <si>
-    <t>atmospheric_temperature</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
-    <t>volume</t>
-  </si>
-  <si>
-    <t>bmi</t>
-  </si>
-  <si>
     <t>meters</t>
   </si>
   <si>
@@ -243,9 +198,6 @@
     <t>The height of XX is 5 meters.</t>
   </si>
   <si>
-    <t>XX weighs 40 kilograms.</t>
-  </si>
-  <si>
     <t>The weight of XX is 40 kilograms.</t>
   </si>
   <si>
@@ -331,13 +283,463 @@
   </si>
   <si>
     <t>xx wants to know the length of the radius of the xx.</t>
+  </si>
+  <si>
+    <t>Complete the function which should return yes if xx has enough money to buy the xx, or no otherwise.</t>
+  </si>
+  <si>
+    <t>Complete the function that returns how many xx can be bought with the money of xx.</t>
+  </si>
+  <si>
+    <t>Complete the function which should return the change xx should receive.</t>
+  </si>
+  <si>
+    <t>Complete the function that computes the body mass index (BMI) of xx.</t>
+  </si>
+  <si>
+    <t>To compute the BMI, divide the weight in kilograms by the height in meters squared.</t>
+  </si>
+  <si>
+    <t>Complete the function the computes for the area of the xx in feet^2.</t>
+  </si>
+  <si>
+    <t>The area of a square is the length of the side squared.</t>
+  </si>
+  <si>
+    <t>The area of a rectangle is the length multiplied by the width.</t>
+  </si>
+  <si>
+    <t>The area of a circle is PI (3.1416) multiplied by the radius squared.</t>
+  </si>
+  <si>
+    <t>Complete the function that returns the radius in feet.</t>
+  </si>
+  <si>
+    <t>Complete the function that converts xx to feet.</t>
+  </si>
+  <si>
+    <t>Complete the function that converts xx to meters.</t>
+  </si>
+  <si>
+    <t>Complete the function that converts xx to kilograms.</t>
+  </si>
+  <si>
+    <t>Complete the function that converts xx to pounds.</t>
+  </si>
+  <si>
+    <t>1 meter is 3.28084 feet.</t>
+  </si>
+  <si>
+    <t>1 kilogram is 2.20462 pounds.</t>
+  </si>
+  <si>
+    <t>Complete the function that converts xx to Fahrenheit.</t>
+  </si>
+  <si>
+    <t>Complete the function that converts xx to Celsius.</t>
+  </si>
+  <si>
+    <t>To convert Celsius to Fahrenheit, multiply it by 9/5 and then add 32.</t>
+  </si>
+  <si>
+    <t>To convert Fahrenheit to Celsius, subtract 32 from it and then multiply it by 5/9.</t>
+  </si>
+  <si>
+    <t>人</t>
+  </si>
+  <si>
+    <t>オーブン</t>
+  </si>
+  <si>
+    <t>靴</t>
+  </si>
+  <si>
+    <t>聴診器</t>
+  </si>
+  <si>
+    <t>野球用バット</t>
+  </si>
+  <si>
+    <t>ラケット</t>
+  </si>
+  <si>
+    <t>本</t>
+  </si>
+  <si>
+    <t>皿</t>
+  </si>
+  <si>
+    <t>画布</t>
+  </si>
+  <si>
+    <t>スケッチブック</t>
+  </si>
+  <si>
+    <t>球</t>
+  </si>
+  <si>
+    <t>食物</t>
+  </si>
+  <si>
+    <t>ピザ</t>
+  </si>
+  <si>
+    <t>ラーメン</t>
+  </si>
+  <si>
+    <t>林檎</t>
+  </si>
+  <si>
+    <t>アメリカ</t>
+  </si>
+  <si>
+    <t>フランス</t>
+  </si>
+  <si>
+    <t>スウェーデン</t>
+  </si>
+  <si>
+    <t>日本</t>
+  </si>
+  <si>
+    <t>食料品</t>
+  </si>
+  <si>
+    <t>レストラン</t>
+  </si>
+  <si>
+    <t>シェフ</t>
+  </si>
+  <si>
+    <t>医師</t>
+  </si>
+  <si>
+    <t>アスリート</t>
+  </si>
+  <si>
+    <t>画家</t>
+  </si>
+  <si>
+    <t>ベーキング</t>
+  </si>
+  <si>
+    <t>料理</t>
+  </si>
+  <si>
+    <t>バスケットボール</t>
+  </si>
+  <si>
+    <t>サッカー</t>
+  </si>
+  <si>
+    <t>テニス</t>
+  </si>
+  <si>
+    <t>バドミントン</t>
+  </si>
+  <si>
+    <t>野球</t>
+  </si>
+  <si>
+    <t>旅行</t>
+  </si>
+  <si>
+    <t>読書</t>
+  </si>
+  <si>
+    <t>絵</t>
+  </si>
+  <si>
+    <t>painting (hobby)</t>
+  </si>
+  <si>
+    <t>eating (hobby)</t>
+  </si>
+  <si>
+    <t>食べる</t>
+  </si>
+  <si>
+    <t>矩形</t>
+  </si>
+  <si>
+    <t>サークル</t>
+  </si>
+  <si>
+    <t>値段</t>
+  </si>
+  <si>
+    <t>お金</t>
+  </si>
+  <si>
+    <t>支払い</t>
+  </si>
+  <si>
+    <t>高さ</t>
+  </si>
+  <si>
+    <t>長さ</t>
+  </si>
+  <si>
+    <t>幅</t>
+  </si>
+  <si>
+    <t>半径</t>
+  </si>
+  <si>
+    <t>直径</t>
+  </si>
+  <si>
+    <t>側</t>
+  </si>
+  <si>
+    <t>height (of person)</t>
+  </si>
+  <si>
+    <t>length (of rectangle)</t>
+  </si>
+  <si>
+    <t>width (of rectangle)</t>
+  </si>
+  <si>
+    <t>radius (of circle)</t>
+  </si>
+  <si>
+    <t>diameter (of circle)</t>
+  </si>
+  <si>
+    <t>side (of square)</t>
+  </si>
+  <si>
+    <t>weight (of person)</t>
+  </si>
+  <si>
+    <t>body_temperature (of person)</t>
+  </si>
+  <si>
+    <t>atmospheric_temperature (of country)</t>
+  </si>
+  <si>
+    <t>体温</t>
+  </si>
+  <si>
+    <t>重量</t>
+  </si>
+  <si>
+    <t>温度</t>
+  </si>
+  <si>
+    <t>エリア</t>
+  </si>
+  <si>
+    <t>bmi (body mass index)</t>
+  </si>
+  <si>
+    <t>メートル</t>
+  </si>
+  <si>
+    <t>フィート</t>
+  </si>
+  <si>
+    <t>キログラム</t>
+  </si>
+  <si>
+    <t>ポンド</t>
+  </si>
+  <si>
+    <t>摂氏</t>
+  </si>
+  <si>
+    <t>華氏</t>
+  </si>
+  <si>
+    <t>メートル法</t>
+  </si>
+  <si>
+    <t>帝国システム</t>
+  </si>
+  <si>
+    <t>晴れた日です。</t>
+  </si>
+  <si>
+    <t>雨の日です。</t>
+  </si>
+  <si>
+    <t>XXはXXです。</t>
+  </si>
+  <si>
+    <t>XXの趣味はXXです。</t>
+  </si>
+  <si>
+    <t>XXはXXを好きです。</t>
+  </si>
+  <si>
+    <t>XXは太りすぎです。</t>
+  </si>
+  <si>
+    <t>XXはもっとフィットしたい。</t>
+  </si>
+  <si>
+    <t>XXは5メートルの高さです。</t>
+  </si>
+  <si>
+    <t>XXの高さは5メートルです。</t>
+  </si>
+  <si>
+    <t>XXの重量は40キロです。</t>
+  </si>
+  <si>
+    <t>XXの体温は摂氏35度です。</t>
+  </si>
+  <si>
+    <t>XXの平均気温は摂氏20度です。</t>
+  </si>
+  <si>
+    <t>1つのXXはXX円かかります。</t>
+  </si>
+  <si>
+    <t>1つのXXの価格はXX円です。</t>
+  </si>
+  <si>
+    <t>XXは合計XX円です。</t>
+  </si>
+  <si>
+    <t>XXは測定にメートル法を使用しています。</t>
+  </si>
+  <si>
+    <t>XXは帝国システムを使用して測定します。</t>
+  </si>
+  <si>
+    <t>XXはXXの形をしています。</t>
+  </si>
+  <si>
+    <t>XXの片側がXXメートルを測定する。</t>
+  </si>
+  <si>
+    <t>XXの半径はXXメートルです。</t>
+  </si>
+  <si>
+    <t>XXの直径はXXメートルです。</t>
+  </si>
+  <si>
+    <t>XXの長さはXXメートルを測定し、XXの幅はXXメートルを測定する。</t>
+  </si>
+  <si>
+    <t>XXは疲れたために空腹感がある。</t>
+  </si>
+  <si>
+    <t>XXはひどく食べたい。</t>
+  </si>
+  <si>
+    <t>XXはXXをする。</t>
+  </si>
+  <si>
+    <t>XXはジムで運動し、疲れました。</t>
+  </si>
+  <si>
+    <t>XXはそのXXに5円を支払った。</t>
+  </si>
+  <si>
+    <t>XXはXXに向かった。</t>
+  </si>
+  <si>
+    <t>XXは雨のために病気になる。</t>
+  </si>
+  <si>
+    <t>XXは新しいXXを購入したい。</t>
+  </si>
+  <si>
+    <t>XXはできるだけ多くのXXを購入したいと考えています。</t>
+  </si>
+  <si>
+    <t>XXは彼が得る変更を決定する必要があります。</t>
+  </si>
+  <si>
+    <t>XXは休暇のためにXXに旅行する予定です。</t>
+  </si>
+  <si>
+    <t>XXはスポーツ競技のためにXXに行くことになります。</t>
+  </si>
+  <si>
+    <t>XXはXXをXXに変換する必要があります。 （例：メートルからフィート）</t>
+  </si>
+  <si>
+    <t>XXは摂氏でXXを知りたい。</t>
+  </si>
+  <si>
+    <t>xxはxxの面積を計算したい。</t>
+  </si>
+  <si>
+    <t>xxはxxの半径の長さを知りたい。</t>
+  </si>
+  <si>
+    <t>xxがxxを購入するのに十分な金額を持っている場合はyesを返し、それ以外の場合はnoを返す関数を完成させます。</t>
+  </si>
+  <si>
+    <t>xxのお金で購入できるxxの数を返す関数を完成させてください。</t>
+  </si>
+  <si>
+    <t>xxが受け取るべき変更を返す関数を完成させてください。</t>
+  </si>
+  <si>
+    <t>xxの体格指数（BMI）を計算する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>体格指数</t>
+  </si>
+  <si>
+    <t>BMIを計算するには、体重を体重（kg）で除します。</t>
+  </si>
+  <si>
+    <t>フィート^ 2でのxxの面積を計算する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>四角形の面積は、四角形の長さです。</t>
+  </si>
+  <si>
+    <t>矩形の面積は、長さに幅を掛けたものです。</t>
+  </si>
+  <si>
+    <t>円の面積はPI（3.1416）に半径の二乗を掛けたものです。</t>
+  </si>
+  <si>
+    <t>半径をフィート単位で返す関数を完成させます。</t>
+  </si>
+  <si>
+    <t>xxをフィートに変換する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>xxをメートルに変換する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>xxをキログラムに変換する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>xxをポンドに変換する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>1メートルは3.28084フィートです。</t>
+  </si>
+  <si>
+    <t>1キログラムは2.20462ポンドです。</t>
+  </si>
+  <si>
+    <t>xxを華氏に変換する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>xxを摂氏に変換する関数を完成させます。</t>
+  </si>
+  <si>
+    <t>摂氏を華氏に変換するには、9/5を掛けて32を加えます。</t>
+  </si>
+  <si>
+    <t>華氏を摂氏に変換するには、摂氏32を引いてから5/9を掛けます。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,13 +747,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -366,8 +785,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,17 +1074,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="92.5703125" customWidth="1"/>
-    <col min="2" max="2" width="62.7109375" customWidth="1"/>
+    <col min="2" max="2" width="134.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -666,517 +1094,952 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B39" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B56" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B57" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B58" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B59" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B60" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B61" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B62" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B63" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B64" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B65" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B66" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B67" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B68" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B69" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B71" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B72" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="B73" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B74" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="B75" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B76" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B77" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="B78" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B79" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B80" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B81" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="B82" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="B83" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="B84" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="B85" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="B86" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="B87" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="B88" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B89" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="B90" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B92" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="B93" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="B94" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="B95" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B96" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="B97" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="B98" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="B99" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B100" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="B101" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B102" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="B103" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="B104" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="B105" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="B106" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B107" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="B108" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B109" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15.75">
+      <c r="A110" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B110" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B111" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B112" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B113" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B114" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
         <v>103</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>104</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>105</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>106</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>107</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>